<commit_message>
Spatial Cross-Validated Super Learner
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAEB06F-AB8C-5F47-9DCD-27CEF39AD430}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B977DCC-36E6-044C-B064-3A638B19E8AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17220" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="113">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>hlthst_nrst_duration_fctb_clst</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Urbanicity</t>
   </si>
 </sst>
 </file>
@@ -946,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO46"/>
+  <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,10 +967,10 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="31" width="10.83203125" style="15"/>
+    <col min="8" max="30" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -986,9 +992,9 @@
       <c r="G1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="15"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE1" s="15"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1004,9 +1010,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="AF2" s="15"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE2" s="15"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1022,9 +1028,9 @@
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="AF3" s="15"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE3" s="15"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1040,9 +1046,9 @@
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="AF4" s="15"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE4" s="15"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1058,9 +1064,9 @@
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="AF5" s="15"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE5" s="15"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1076,9 +1082,9 @@
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="AF6" s="15"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE6" s="15"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1094,9 +1100,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="AF7" s="15"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE7" s="15"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1112,9 +1118,9 @@
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="AF8" s="15"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE8" s="15"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1130,14 +1136,14 @@
       <c r="E9" s="3"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="AF9" s="15"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE9" s="15"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>57</v>
@@ -1148,14 +1154,14 @@
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="AF10" s="15"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE10" s="15"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>109</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>57</v>
@@ -1163,16 +1169,18 @@
       <c r="D11" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="F11" s="14" t="s">
         <v>63</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="15"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE11" s="15"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>106</v>
       </c>
@@ -1190,9 +1198,9 @@
         <v>63</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="AF12" s="15"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE12" s="15"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>107</v>
       </c>
@@ -1206,13 +1214,11 @@
         <v>49</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="AF13" s="15"/>
-    </row>
-    <row r="14" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE13" s="15"/>
+    </row>
+    <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>105</v>
       </c>
@@ -1230,9 +1236,9 @@
       <c r="G14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF14" s="15"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE14" s="15"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>108</v>
       </c>
@@ -1247,12 +1253,10 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF15" s="15"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="G15" s="8"/>
+      <c r="AE15" s="15"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1270,9 +1274,9 @@
         <v>63</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="AF16" s="15"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE16" s="15"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -1290,9 +1294,9 @@
       <c r="G17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF17" s="15"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE17" s="15"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
@@ -1310,9 +1314,9 @@
         <v>63</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="AF18" s="15"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE18" s="15"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>94</v>
       </c>
@@ -1330,9 +1334,9 @@
       <c r="G19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF19" s="15"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE19" s="15"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>110</v>
       </c>
@@ -1352,9 +1356,9 @@
       <c r="G20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF20" s="15"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE20" s="15"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>101</v>
       </c>
@@ -1372,9 +1376,9 @@
         <v>63</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="AF21" s="15"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE21" s="15"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -1392,9 +1396,9 @@
       <c r="G22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF22" s="15"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE22" s="15"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
@@ -1414,9 +1418,9 @@
         <v>63</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="AF23" s="15"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE23" s="15"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
@@ -1434,9 +1438,9 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="AF24" s="15"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE24" s="15"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
@@ -1454,9 +1458,9 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="AF25" s="15"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE25" s="15"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>97</v>
       </c>
@@ -1478,9 +1482,9 @@
       <c r="G26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF26" s="15"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE26" s="15"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1502,9 +1506,9 @@
       <c r="G27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF27" s="15"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE27" s="15"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1522,9 +1526,9 @@
         <v>63</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="AF28" s="15"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE28" s="15"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1542,9 +1546,9 @@
       <c r="G29" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF29" s="15"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE29" s="15"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1566,9 +1570,9 @@
       <c r="G30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF30" s="15"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE30" s="15"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>93</v>
       </c>
@@ -1590,9 +1594,9 @@
       <c r="G31" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF31" s="15"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AE31" s="15"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>69</v>
       </c>
@@ -1614,9 +1618,9 @@
       <c r="G32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF32" s="15"/>
-    </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE32" s="15"/>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
@@ -1638,9 +1642,9 @@
       <c r="G33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF33" s="15"/>
-    </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE33" s="15"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>14</v>
       </c>
@@ -1658,9 +1662,9 @@
         <v>63</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="AF34" s="15"/>
-    </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE34" s="15"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -1678,9 +1682,9 @@
       <c r="G35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF35" s="15"/>
-    </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE35" s="15"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>70</v>
       </c>
@@ -1702,9 +1706,9 @@
       <c r="G36" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AF36" s="15"/>
-    </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE36" s="15"/>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>27</v>
       </c>
@@ -1720,9 +1724,9 @@
       <c r="E37" s="4"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="AF37" s="15"/>
-    </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE37" s="15"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>28</v>
       </c>
@@ -1738,9 +1742,9 @@
       <c r="E38" s="4"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="AF38" s="15"/>
-    </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE38" s="15"/>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>29</v>
       </c>
@@ -1756,9 +1760,9 @@
       <c r="E39" s="4"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="AF39" s="15"/>
-    </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE39" s="15"/>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>30</v>
       </c>
@@ -1774,9 +1778,9 @@
       <c r="E40" s="4"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
-      <c r="AF40" s="15"/>
-    </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE40" s="15"/>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>0</v>
       </c>
@@ -1792,9 +1796,9 @@
       <c r="E41" s="11"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
-      <c r="AF41" s="15"/>
-    </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE41" s="15"/>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>1</v>
       </c>
@@ -1810,9 +1814,9 @@
       <c r="E42" s="11"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
-      <c r="AF42" s="15"/>
-    </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE42" s="15"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>2</v>
       </c>
@@ -1828,9 +1832,9 @@
       <c r="E43" s="11"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
-      <c r="AF43" s="15"/>
-    </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE43" s="15"/>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>3</v>
       </c>
@@ -1846,9 +1850,9 @@
       <c r="E44" s="11"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-      <c r="AF44" s="15"/>
-    </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE44" s="15"/>
+    </row>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>4</v>
       </c>
@@ -1864,9 +1868,9 @@
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="AF45" s="15"/>
-    </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AE45" s="15"/>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>5</v>
       </c>
@@ -1882,7 +1886,8 @@
       <c r="E46" s="11"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-      <c r="AF46" s="15"/>
+      <c r="AE46" s="15"/>
+      <c r="AF46" s="4"/>
       <c r="AG46" s="4"/>
       <c r="AH46" s="4"/>
       <c r="AI46" s="4"/>
@@ -1891,7 +1896,6 @@
       <c r="AL46" s="4"/>
       <c r="AM46" s="4"/>
       <c r="AN46" s="4"/>
-      <c r="AO46" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
update power and covar functions
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEA27E9-16C3-B24B-B027-39C2CC8FF1CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258C61BD-858F-BA4A-A448-6A94C8719153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="1420" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
update superlearner and prevmap codes
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258C61BD-858F-BA4A-A448-6A94C8719153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C938E5-CD15-8847-B691-A413FD90BDD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1420" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -204,9 +204,6 @@
     <t>survey month year lagged</t>
   </si>
   <si>
-    <t>urban vs rural original coding</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>hivpos</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
     <t>urban_rura_fctb</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>Urbanicity</t>
   </si>
   <si>
@@ -370,6 +361,9 @@
   </si>
   <si>
     <t>farmer</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -948,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,19 +966,19 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="AE1" s="15"/>
     </row>
@@ -999,7 +993,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
@@ -1017,7 +1011,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -1035,7 +1029,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
@@ -1053,7 +1047,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
@@ -1071,7 +1065,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
@@ -1089,7 +1083,7 @@
         <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
@@ -1107,7 +1101,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
@@ -1125,7 +1119,7 @@
         <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="9"/>
@@ -1137,13 +1131,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
@@ -1152,77 +1146,77 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE11" s="15"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" s="8"/>
       <c r="AE12" s="15"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="8"/>
       <c r="AE13" s="15"/>
     </row>
     <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>47</v>
@@ -1230,28 +1224,26 @@
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE14" s="15"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="G15" s="8"/>
       <c r="AE15" s="15"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
@@ -1269,14 +1261,14 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="8"/>
       <c r="AE16" s="15"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>46</v>
@@ -1290,39 +1282,39 @@
       <c r="E17" s="2"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE17" s="15"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="8"/>
       <c r="AE18" s="15"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>47</v>
@@ -1330,61 +1322,61 @@
       <c r="E19" s="2"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE19" s="15"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE20" s="15"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G21" s="8"/>
       <c r="AE21" s="15"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>47</v>
@@ -1392,7 +1384,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE22" s="15"/>
     </row>
@@ -1404,16 +1396,16 @@
         <v>35</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" s="7"/>
       <c r="AE23" s="15"/>
@@ -1426,13 +1418,13 @@
         <v>36</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -1446,43 +1438,43 @@
         <v>37</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE25" s="15"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE26" s="15"/>
     </row>
@@ -1500,13 +1492,13 @@
         <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE27" s="15"/>
     </row>
@@ -1525,7 +1517,7 @@
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G28" s="7"/>
       <c r="AE28" s="15"/>
@@ -1546,31 +1538,31 @@
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE29" s="15"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE30" s="15"/>
     </row>
@@ -1579,28 +1571,28 @@
         <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE31" s="15"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>40</v>
@@ -1613,16 +1605,16 @@
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE32" s="15"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>41</v>
@@ -1635,10 +1627,10 @@
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE33" s="15"/>
     </row>
@@ -1650,14 +1642,14 @@
         <v>42</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" s="7"/>
       <c r="AE34" s="15"/>
@@ -1670,7 +1662,7 @@
         <v>42</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>45</v>
@@ -1678,31 +1670,31 @@
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE35" s="15"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE36" s="15"/>
     </row>
@@ -1711,13 +1703,13 @@
         <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="10"/>
@@ -1729,13 +1721,13 @@
         <v>27</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="10"/>
@@ -1753,7 +1745,7 @@
         <v>28</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="10"/>
@@ -1765,13 +1757,13 @@
         <v>29</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="10"/>
@@ -1789,7 +1781,7 @@
         <v>33</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="12"/>
@@ -1807,7 +1799,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="12"/>
@@ -1825,7 +1817,7 @@
         <v>32</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="12"/>
@@ -1843,7 +1835,7 @@
         <v>32</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="12"/>
@@ -1861,7 +1853,7 @@
         <v>34</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
@@ -1879,7 +1871,7 @@
         <v>34</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="12"/>
@@ -1926,7 +1918,7 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update prevmap work and start tidy
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C938E5-CD15-8847-B691-A413FD90BDD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1FE005-30FD-E54E-B250-8D00D3FAEA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1420" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="1340" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covars" sheetId="1" r:id="rId1"/>
@@ -37,25 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
-  <si>
-    <t>pfldhct_cont</t>
-  </si>
-  <si>
-    <t>pfldhct_cont_log</t>
-  </si>
-  <si>
-    <t>po18sct_cont</t>
-  </si>
-  <si>
-    <t>po18sct_cont_log</t>
-  </si>
-  <si>
-    <t>pv18sct_cont</t>
-  </si>
-  <si>
-    <t>pv18sct_cont_log</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -123,9 +105,6 @@
     <t>longnum</t>
   </si>
   <si>
-    <t>geometry</t>
-  </si>
-  <si>
     <t>adm1name</t>
   </si>
   <si>
@@ -135,15 +114,6 @@
     <t>var_label</t>
   </si>
   <si>
-    <t>Ovale CT</t>
-  </si>
-  <si>
-    <t>Falciparum CT</t>
-  </si>
-  <si>
-    <t>Vivax CT</t>
-  </si>
-  <si>
     <t>Falciparum infxn</t>
   </si>
   <si>
@@ -232,9 +202,6 @@
   </si>
   <si>
     <t>alt_dem_cont_scale_clst</t>
-  </si>
-  <si>
-    <t>sens</t>
   </si>
   <si>
     <t>ITN_fctb</t>
@@ -424,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,12 +419,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,7 +464,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -517,11 +478,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -625,10 +584,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G46" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:G49">
-    <sortCondition ref="D1:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G39" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:G39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:G42">
+    <sortCondition ref="D1:D42"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
@@ -940,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN46"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,937 +914,802 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="30" width="10.83203125" style="15"/>
+    <col min="8" max="30" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="AE1" s="13"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="AE2" s="15"/>
+      <c r="AE2" s="13"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="AE3" s="15"/>
+      <c r="AE3" s="13"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="AE4" s="15"/>
+      <c r="AE4" s="13"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="AE5" s="15"/>
+      <c r="AE5" s="13"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="AE6" s="15"/>
+      <c r="AE6" s="13"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="AE7" s="15"/>
+      <c r="AE7" s="13"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="AE8" s="15"/>
+      <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="AE9" s="15"/>
+      <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="AE10" s="13"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="AE10" s="15"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE11" s="15"/>
+      <c r="F11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="AE12" s="15"/>
+      <c r="AE12" s="13"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="AE13" s="15"/>
+      <c r="AE13" s="13"/>
     </row>
     <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE14" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="AE15" s="15"/>
+      <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="AE16" s="15"/>
+      <c r="AE16" s="13"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE17" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE17" s="13"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="AE18" s="15"/>
+      <c r="AE18" s="13"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE19" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE19" s="13"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>100</v>
+      <c r="A20" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE20" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE20" s="13"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="AE21" s="15"/>
+      <c r="AE21" s="13"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE22" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE22" s="13"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="AE23" s="15"/>
+      <c r="AE23" s="13"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>83</v>
+        <v>26</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="AE24" s="15"/>
+      <c r="AE24" s="13"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE25" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE25" s="13"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE26" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE26" s="13"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE27" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE27" s="13"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="AE28" s="15"/>
+      <c r="AE28" s="13"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE29" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE29" s="13"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE30" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE30" s="13"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE31" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE32" s="15"/>
-    </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="AE32" s="13"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE33" s="15"/>
-    </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="AE33" s="13"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="AE34" s="15"/>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AE34" s="13"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE35" s="15"/>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="AE35" s="13"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE36" s="13"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE36" s="15"/>
-    </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="C37" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="AE37" s="15"/>
-    </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AE37" s="13"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="AE38" s="15"/>
-    </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AE38" s="13"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="AE39" s="15"/>
-    </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="AE40" s="15"/>
-    </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="AE41" s="15"/>
-    </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="AE42" s="15"/>
-    </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="AE43" s="15"/>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="AE44" s="15"/>
-    </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="AE45" s="15"/>
-    </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="AE46" s="15"/>
-      <c r="AF46" s="4"/>
-      <c r="AG46" s="4"/>
-      <c r="AH46" s="4"/>
-      <c r="AI46" s="4"/>
-      <c r="AJ46" s="4"/>
-      <c r="AK46" s="4"/>
-      <c r="AL46" s="4"/>
-      <c r="AM46" s="4"/>
-      <c r="AN46" s="4"/>
+      <c r="AE39" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1909,16 +1733,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add various featues for plotting and for prevmap not working well on LL
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E53E32-4803-3E4A-AE94-4DCF1811641C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89395A7F-65BE-DC48-BCCA-6447EA76D60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1340" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -246,15 +246,6 @@
     <t>Water Dist.</t>
   </si>
   <si>
-    <t xml:space="preserve">P. falciparum </t>
-  </si>
-  <si>
-    <t>P. vivax</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
     <t>Num. House-Members</t>
   </si>
   <si>
@@ -316,6 +307,24 @@
   </si>
   <si>
     <t>near</t>
+  </si>
+  <si>
+    <t>Sex (Male)</t>
+  </si>
+  <si>
+    <t>HIV (+)</t>
+  </si>
+  <si>
+    <t>P. falciparum (+)</t>
+  </si>
+  <si>
+    <t>P. vivax (+)</t>
+  </si>
+  <si>
+    <t>ITN Use (No)</t>
+  </si>
+  <si>
+    <t>Housing Materials (Trad.)</t>
   </si>
 </sst>
 </file>
@@ -886,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,10 +1084,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>48</v>
@@ -1090,19 +1099,19 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>50</v>
@@ -1114,10 +1123,10 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>66</v>
@@ -1134,10 +1143,10 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>67</v>
@@ -1154,10 +1163,10 @@
     </row>
     <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>66</v>
@@ -1174,10 +1183,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>67</v>
@@ -1232,7 +1241,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>53</v>
@@ -1244,7 +1253,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>50</v>
@@ -1256,19 +1265,19 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>50</v>
@@ -1286,7 +1295,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>35</v>
@@ -1308,7 +1317,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>35</v>
@@ -1328,7 +1337,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>35</v>
@@ -1352,7 +1361,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>35</v>
@@ -1410,19 +1419,19 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>50</v>
@@ -1440,7 +1449,7 @@
         <v>57</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>35</v>
@@ -1458,7 +1467,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -1480,7 +1489,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>31</v>
@@ -1508,7 +1517,7 @@
         <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>35</v>
@@ -1528,7 +1537,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>35</v>
@@ -1548,7 +1557,7 @@
         <v>56</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
add various features for plotting and for prevmap not working on LL
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E53E32-4803-3E4A-AE94-4DCF1811641C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89395A7F-65BE-DC48-BCCA-6447EA76D60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1340" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -246,15 +246,6 @@
     <t>Water Dist.</t>
   </si>
   <si>
-    <t xml:space="preserve">P. falciparum </t>
-  </si>
-  <si>
-    <t>P. vivax</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
     <t>Num. House-Members</t>
   </si>
   <si>
@@ -316,6 +307,24 @@
   </si>
   <si>
     <t>near</t>
+  </si>
+  <si>
+    <t>Sex (Male)</t>
+  </si>
+  <si>
+    <t>HIV (+)</t>
+  </si>
+  <si>
+    <t>P. falciparum (+)</t>
+  </si>
+  <si>
+    <t>P. vivax (+)</t>
+  </si>
+  <si>
+    <t>ITN Use (No)</t>
+  </si>
+  <si>
+    <t>Housing Materials (Trad.)</t>
   </si>
 </sst>
 </file>
@@ -886,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,10 +1084,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>48</v>
@@ -1090,19 +1099,19 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>50</v>
@@ -1114,10 +1123,10 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>66</v>
@@ -1134,10 +1143,10 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>67</v>
@@ -1154,10 +1163,10 @@
     </row>
     <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>66</v>
@@ -1174,10 +1183,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>67</v>
@@ -1232,7 +1241,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>53</v>
@@ -1244,7 +1253,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>50</v>
@@ -1256,19 +1265,19 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>50</v>
@@ -1286,7 +1295,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>35</v>
@@ -1308,7 +1317,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>35</v>
@@ -1328,7 +1337,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>35</v>
@@ -1352,7 +1361,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>35</v>
@@ -1410,19 +1419,19 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>50</v>
@@ -1440,7 +1449,7 @@
         <v>57</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>35</v>
@@ -1458,7 +1467,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -1480,7 +1489,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>31</v>
@@ -1508,7 +1517,7 @@
         <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>35</v>
@@ -1528,7 +1537,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>35</v>
@@ -1548,7 +1557,7 @@
         <v>56</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
subset to de jure. tidy up for reproducibility
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D266F57-7581-294B-BF01-C6104EED0B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A16F23D-048F-4F41-BF15-37DE08182091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1340" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -81,9 +81,6 @@
     <t>hv005</t>
   </si>
   <si>
-    <t>hv005_wi</t>
-  </si>
-  <si>
     <t>houseid</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>hvyrmnth_dtmnth</t>
   </si>
   <si>
-    <t>hvyrmnth_dtmnth_lag</t>
-  </si>
-  <si>
     <t>urban_rura</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>survey month year</t>
   </si>
   <si>
-    <t>survey month year lagged</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -328,6 +319,9 @@
   </si>
   <si>
     <t>Urbanicity (Rur.)</t>
+  </si>
+  <si>
+    <t>hiv05_wi</t>
   </si>
 </sst>
 </file>
@@ -581,10 +575,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G35" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:G35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:G38">
-    <sortCondition ref="D1:D38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:G34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:G37">
+    <sortCondition ref="D1:D37"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
@@ -896,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,25 +910,25 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE1" s="13"/>
     </row>
@@ -943,13 +937,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
@@ -961,13 +955,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -979,13 +973,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
@@ -994,16 +988,16 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
@@ -1012,16 +1006,16 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
@@ -1030,16 +1024,16 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
@@ -1048,16 +1042,16 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
@@ -1065,529 +1059,529 @@
       <c r="AE8" s="13"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="AE9" s="13"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="AE10" s="13"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="8"/>
       <c r="AE11" s="13"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="8"/>
       <c r="AE12" s="13"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="AE13" s="13"/>
     </row>
-    <row r="14" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="G14" s="8"/>
       <c r="AE14" s="13"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="AE15" s="13"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="AE16" s="13"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G17" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE17" s="13"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>88</v>
+      <c r="A18" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE18" s="13"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE18" s="13"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="D19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="7"/>
       <c r="AE19" s="13"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>50</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="AE20" s="13"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>93</v>
+        <v>25</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="AE21" s="13"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE22" s="13"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G23" s="7"/>
       <c r="AE23" s="13"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="AE24" s="13"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE25" s="13"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE26" s="13"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>63</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE27" s="13"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE28" s="13"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G29" s="7"/>
       <c r="AE29" s="13"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="AE30" s="13"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="G31" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE31" s="13"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="A32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
       <c r="AE32" s="13"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="10"/>
@@ -1596,39 +1590,21 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="AE34" s="13"/>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="AE35" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1655,13 +1631,13 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spatial preds for hlthdist
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D11A6C5-95F5-664C-9768-828E5388C4C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD464FFF-0814-9A46-B22E-9E1F9C468DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="5700" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -224,12 +224,6 @@
   </si>
   <si>
     <t>Num. House-Members</t>
-  </si>
-  <si>
-    <t>Lagged Precipitation</t>
-  </si>
-  <si>
-    <t>Lagged Temperature</t>
   </si>
   <si>
     <t>precip_mean_cont_scale_clst</t>
@@ -894,7 +888,7 @@
   <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,13 +929,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
@@ -989,13 +983,13 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1007,13 +1001,13 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
@@ -1082,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>42</v>
@@ -1097,19 +1091,19 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>44</v>
@@ -1121,10 +1115,10 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>60</v>
@@ -1141,10 +1135,10 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>60</v>
@@ -1161,10 +1155,10 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>61</v>
@@ -1181,10 +1175,10 @@
     </row>
     <row r="15" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>61</v>
@@ -1241,7 +1235,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>47</v>
@@ -1261,7 +1255,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>47</v>
@@ -1281,19 +1275,19 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>44</v>
@@ -1311,7 +1305,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>32</v>
@@ -1331,7 +1325,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>32</v>
@@ -1351,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>32</v>
@@ -1375,7 +1369,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>32</v>
@@ -1433,19 +1427,19 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>44</v>
@@ -1463,7 +1457,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>32</v>
@@ -1481,7 +1475,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -1503,7 +1497,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>28</v>
@@ -1515,7 +1509,7 @@
         <v>32</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>44</v>
@@ -1573,7 +1567,7 @@
         <v>50</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
fix urban for figure
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD464FFF-0814-9A46-B22E-9E1F9C468DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A433721-39BB-BB45-BB79-39161EB5F659}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="5700" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>farmer</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>Sex (Male)</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>far</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
   <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,13 +929,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
@@ -983,13 +983,13 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
@@ -1097,13 +1097,13 @@
         <v>69</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>44</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>47</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>47</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>70</v>
@@ -1287,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>44</v>
@@ -1305,7 +1305,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>32</v>
@@ -1325,7 +1325,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>32</v>
@@ -1345,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>32</v>
@@ -1369,7 +1369,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>32</v>
@@ -1457,7 +1457,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>32</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>28</v>
@@ -1509,7 +1509,7 @@
         <v>32</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>44</v>
@@ -1567,7 +1567,7 @@
         <v>50</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
make the sub_decoder have the labels we want for better x-axis figures
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A0D3F5-F684-7748-88E3-92CC30B3CCB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C43C0A-FD7B-A644-BC0C-4AE0D569B1FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="1940" windowWidth="21220" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="97">
   <si>
     <t>pfldh_fctb</t>
   </si>
@@ -247,9 +247,6 @@
     <t xml:space="preserve">Distance to Nearest Public Hospital </t>
   </si>
   <si>
-    <t>Hospital Dist.</t>
-  </si>
-  <si>
     <t>farmer_fctb</t>
   </si>
   <si>
@@ -317,6 +314,15 @@
   </si>
   <si>
     <t>poor</t>
+  </si>
+  <si>
+    <t>Hospital Dist. (Far)</t>
+  </si>
+  <si>
+    <t>Wealth (Poor)</t>
+  </si>
+  <si>
+    <t>Education (Lower)</t>
   </si>
 </sst>
 </file>
@@ -888,7 +894,7 @@
   <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,13 +935,13 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
@@ -983,13 +989,13 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
@@ -1001,13 +1007,13 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>42</v>
@@ -1103,7 +1109,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>44</v>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>47</v>
@@ -1255,7 +1261,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>47</v>
@@ -1275,19 +1281,19 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>44</v>
@@ -1305,7 +1311,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>32</v>
@@ -1325,7 +1331,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>32</v>
@@ -1345,7 +1351,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>32</v>
@@ -1369,7 +1375,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>32</v>
@@ -1427,19 +1433,19 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>44</v>
@@ -1457,7 +1463,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>32</v>
@@ -1475,19 +1481,19 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>44</v>
@@ -1499,19 +1505,19 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>44</v>
@@ -1569,7 +1575,7 @@
         <v>50</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>32</v>

</xml_diff>